<commit_message>
Updated with review Comments
</commit_message>
<xml_diff>
--- a/Traceability matrix.xlsx
+++ b/Traceability matrix.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Elsa\project notes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Elsa\TechChallenge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C3837F0D-0F19-4F77-A5C6-213301C0D14F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CC5DEE8-72BA-4D2F-8950-D0D497FE8483}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{7A617AB5-6400-4CD2-BCB1-CFBE8878970A}"/>
   </bookViews>
@@ -18,7 +18,6 @@
     <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>As the Clerk, I should be able to upload a csv file to a portal so
 that I can populate the database from a UI
@@ -94,21 +93,6 @@
 (natid), Name, Gender, Birthday, Salary and Tax paid</t>
   </si>
   <si>
-    <t>AC1:Postman
-AC2:Scenario: To check the natid field is masked from the 5th character onwards
-AC3,4,5,6:To chek the taxrelief amount verification for the records with 24 test data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-LandingPage.feature
-TC1:Scenario: To check the CSV fileupload function with a valid data.AUTOIT script is used to select the file.The files should be placed in "C:\Test" folder
-Uploading data1.csv file with records.
-The number of records in the csv file must be same in the validate code
-TC2:Scenario: To check the CSV fileupload function with an invalid data
-Uploading data2.csv file with records.
-The number of records in the csv file must be same in the validate code</t>
-  </si>
-  <si>
     <t>USerStory2</t>
   </si>
   <si>
@@ -117,10 +101,6 @@
 AC1: Enhancement of (1), with the ability to insert a list</t>
   </si>
   <si>
-    <t>LandingPage.feature
-Scenario: To check the Displense Now button availability and the functionality</t>
-  </si>
-  <si>
     <t>User Story#</t>
   </si>
   <si>
@@ -131,22 +111,6 @@
   </si>
   <si>
     <t>TestData</t>
-  </si>
-  <si>
-    <t>Postman collection-InsertUser Collection.</t>
-  </si>
-  <si>
-    <t>Postman collection-MultipleUser collection</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Run using newman
-newman run InsertUser.json
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Run using newman
-newman run InsertUser.json -d data1.csv
-</t>
   </si>
   <si>
     <t>Run Options</t>
@@ -160,6 +124,33 @@
 Set Goal:test
 4.Click Run button
 </t>
+  </si>
+  <si>
+    <t>SingleUserInsertAPI.feature</t>
+  </si>
+  <si>
+    <t>MultipleInsertionAPI.feature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+AutoUploadCSVFile.feature
+TC1:Scenario: To check the CSV fileupload function with a valid data.AUTOIT script is used to select the file.The files should be placed in "C:\Test" folder
+Uploading data1.csv file with records.
+The number of records in the csv file must be same in the validate code
+TC2:Scenario: To check the CSV fileupload function with an invalid data
+Uploading data2.csv file with records.
+The number of records in the csv file must be same in the validate code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+AC1:GetTaxReliefAPI.feature
+TaxCalculation.feature
+AC2:Scenario: To check the natid field is masked from the 5th character onwards
+AC3,4,5,6:To chek the taxrelief amount verification for the records with 24 test data</t>
+  </si>
+  <si>
+    <t>DispenseNow.feature
+Scenario: To check the Displense Now button availability and the functionality</t>
   </si>
 </sst>
 </file>
@@ -329,61 +320,6 @@
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
                   <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-            </a:solidFill>
-            <a:ln w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a:ln>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>3</xdr:col>
-          <xdr:colOff>298450</xdr:colOff>
-          <xdr:row>2</xdr:row>
-          <xdr:rowOff>50800</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>3</xdr:col>
-          <xdr:colOff>1212850</xdr:colOff>
-          <xdr:row>2</xdr:row>
-          <xdr:rowOff>431800</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1029" name="Object 5" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1029"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -717,7 +653,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5320624B-5781-4948-8889-60A01AEC87B9}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E4" sqref="E4:E6"/>
     </sheetView>
   </sheetViews>
@@ -731,19 +667,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>14</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="58" x14ac:dyDescent="0.35">
@@ -754,27 +690,23 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
       <c r="D3" s="1"/>
-      <c r="E3" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" ht="173.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -784,11 +716,11 @@
         <v>0</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="6" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="2" customFormat="1" ht="261" x14ac:dyDescent="0.35">
@@ -799,7 +731,7 @@
         <v>5</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="E5" s="7"/>
     </row>
@@ -811,7 +743,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E6" s="7"/>
     </row>
@@ -874,31 +806,6 @@
         <oleObject progId="Macro-Enabled Worksheet" dvAspect="DVASPECT_ICON" shapeId="1026" r:id="rId6"/>
       </mc:Fallback>
     </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <oleObject progId="Macro-Enabled Worksheet" dvAspect="DVASPECT_ICON" shapeId="1029" r:id="rId8">
-          <objectPr defaultSize="0" autoPict="0" r:id="rId5">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>298450</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>50800</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>1212850</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>431800</xdr:rowOff>
-              </to>
-            </anchor>
-          </objectPr>
-        </oleObject>
-      </mc:Choice>
-      <mc:Fallback>
-        <oleObject progId="Macro-Enabled Worksheet" dvAspect="DVASPECT_ICON" shapeId="1029" r:id="rId8"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
   </oleObjects>
 </worksheet>
 </file>

</xml_diff>